<commit_message>
Observed non-replicated nodes filtered out from posterior/prior update in SVB
</commit_message>
<xml_diff>
--- a/extensions/ida2016/doc-Experiments/ExperimentsResults.xlsx
+++ b/extensions/ida2016/doc-Experiments/ExperimentsResults.xlsx
@@ -710,11 +710,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2102297416"/>
-        <c:axId val="2102299704"/>
+        <c:axId val="-2141073096"/>
+        <c:axId val="-2120873816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2102297416"/>
+        <c:axId val="-2141073096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -723,7 +723,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102299704"/>
+        <c:crossAx val="-2120873816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -731,7 +731,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2102299704"/>
+        <c:axId val="-2120873816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -742,7 +742,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102297416"/>
+        <c:crossAx val="-2141073096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1062,11 +1062,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2102480760"/>
-        <c:axId val="2102477992"/>
+        <c:axId val="-2120462728"/>
+        <c:axId val="-2141278408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2102480760"/>
+        <c:axId val="-2120462728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1075,7 +1075,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102477992"/>
+        <c:crossAx val="-2141278408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1083,7 +1083,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2102477992"/>
+        <c:axId val="-2141278408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1094,14 +1094,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102480760"/>
+        <c:crossAx val="-2120462728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1415,11 +1414,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2102371288"/>
-        <c:axId val="2102374248"/>
+        <c:axId val="-2122064472"/>
+        <c:axId val="-2122061528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2102371288"/>
+        <c:axId val="-2122064472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1428,7 +1427,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102374248"/>
+        <c:crossAx val="-2122061528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1436,7 +1435,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2102374248"/>
+        <c:axId val="-2122061528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,14 +1446,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102371288"/>
+        <c:crossAx val="-2122064472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1763,11 +1761,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2102457144"/>
-        <c:axId val="2102447640"/>
+        <c:axId val="2064679000"/>
+        <c:axId val="-2120035688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2102457144"/>
+        <c:axId val="2064679000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1776,7 +1774,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102447640"/>
+        <c:crossAx val="-2120035688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1784,7 +1782,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2102447640"/>
+        <c:axId val="-2120035688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1795,14 +1793,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102457144"/>
+        <c:crossAx val="2064679000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2111,11 +2108,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2114535704"/>
-        <c:axId val="-2139793624"/>
+        <c:axId val="-2122011352"/>
+        <c:axId val="-2122008408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2114535704"/>
+        <c:axId val="-2122011352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2124,7 +2121,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139793624"/>
+        <c:crossAx val="-2122008408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2132,7 +2129,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2139793624"/>
+        <c:axId val="-2122008408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2143,14 +2140,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114535704"/>
+        <c:crossAx val="-2122011352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2719,11 +2715,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2054310104"/>
-        <c:axId val="2054307144"/>
+        <c:axId val="-2120342920"/>
+        <c:axId val="-2142131384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2054310104"/>
+        <c:axId val="-2120342920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2732,7 +2728,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2054307144"/>
+        <c:crossAx val="-2142131384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2740,7 +2736,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2054307144"/>
+        <c:axId val="-2142131384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2751,14 +2747,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2054310104"/>
+        <c:crossAx val="-2120342920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3072,11 +3067,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2054282328"/>
-        <c:axId val="2054279640"/>
+        <c:axId val="2112886264"/>
+        <c:axId val="-2120900104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2054282328"/>
+        <c:axId val="2112886264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3085,7 +3080,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2054279640"/>
+        <c:crossAx val="-2120900104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3093,7 +3088,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2054279640"/>
+        <c:axId val="-2120900104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3104,14 +3099,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2054282328"/>
+        <c:crossAx val="2112886264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3159,253 +3153,253 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
                 <c:pt idx="0">
-                  <c:v>3725.88314900197</c:v>
+                  <c:v>2471.90801716197</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3725.89250120852</c:v>
+                  <c:v>2471.90761420583</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4400.71939631046</c:v>
+                  <c:v>2832.10534763796</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4041.85111196139</c:v>
+                  <c:v>2946.31433087394</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3977.01753281747</c:v>
+                  <c:v>2937.66150265199</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4198.16108367076</c:v>
+                  <c:v>2988.00728319054</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4214.72542118552</c:v>
+                  <c:v>2592.05108821683</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4144.01158251411</c:v>
+                  <c:v>2583.54032601889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4797.17460007536</c:v>
+                  <c:v>2992.11608545052</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4258.31975480517</c:v>
+                  <c:v>3458.5313264306</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4214.05126407202</c:v>
+                  <c:v>3447.33488704491</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4309.3284046932</c:v>
+                  <c:v>3502.62278615308</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4284.39878664705</c:v>
+                  <c:v>4550.85080605488</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4255.23131266102</c:v>
+                  <c:v>4530.88196303332</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4988.96130094833</c:v>
+                  <c:v>5335.5759672632</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4363.87660392262</c:v>
+                  <c:v>5721.05160063247</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4250.76133416055</c:v>
+                  <c:v>5604.39671980428</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4323.99197791217</c:v>
+                  <c:v>5734.85754494854</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4336.74406177185</c:v>
+                  <c:v>6539.66664704828</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4281.14370771661</c:v>
+                  <c:v>6540.23183578467</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5040.03396070909</c:v>
+                  <c:v>7765.90785261664</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4323.90265980392</c:v>
+                  <c:v>6537.44233175773</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4345.35097909005</c:v>
+                  <c:v>6530.894734381</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4416.97648459526</c:v>
+                  <c:v>6657.72355583749</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4395.10999915062</c:v>
+                  <c:v>7248.25315023225</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4382.53920715789</c:v>
+                  <c:v>7215.36465847751</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5124.29210336257</c:v>
+                  <c:v>8457.882289220361</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4896.23410756647</c:v>
+                  <c:v>8119.62280147059</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4659.66430010356</c:v>
+                  <c:v>8159.0324143647</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4773.17789942186</c:v>
+                  <c:v>8371.568993003561</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4639.25048067069</c:v>
+                  <c:v>6568.32265213683</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4648.67817722821</c:v>
+                  <c:v>6522.33073546855</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5524.30218376842</c:v>
+                  <c:v>7851.93046757931</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4714.02271060908</c:v>
+                  <c:v>7523.35216718273</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4693.66673775213</c:v>
+                  <c:v>7453.36797626202</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4898.95581048953</c:v>
+                  <c:v>7696.23800027293</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4778.27944633698</c:v>
+                  <c:v>7919.28856588064</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4782.61632193142</c:v>
+                  <c:v>7954.15612303297</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5644.83949894361</c:v>
+                  <c:v>9507.989128763609</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4826.61687036336</c:v>
+                  <c:v>7446.64620151523</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4778.39416705253</c:v>
+                  <c:v>7477.33992408778</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4820.71842677897</c:v>
+                  <c:v>7613.03373485845</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4734.3769846949</c:v>
+                  <c:v>7323.17121275802</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4706.7448758225</c:v>
+                  <c:v>7386.98066700287</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>5619.79781996368</c:v>
+                  <c:v>8882.278987636</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4819.2510926942</c:v>
+                  <c:v>8826.467806617309</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4784.21293640808</c:v>
+                  <c:v>8745.925389632381</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>5644.30603176369</c:v>
+                  <c:v>10505.3051095258</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4794.48243949468</c:v>
+                  <c:v>9595.52285115677</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4798.9647724515</c:v>
+                  <c:v>9663.36865260388</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>5658.5114680776</c:v>
+                  <c:v>11627.7200705803</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>4852.73540301032</c:v>
+                  <c:v>9832.045539705199</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4707.22922693011</c:v>
+                  <c:v>9654.42337983741</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>5591.23926965294</c:v>
+                  <c:v>11724.8489980831</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4779.49489716019</c:v>
+                  <c:v>9236.16526863055</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>4743.97272167656</c:v>
+                  <c:v>9196.73381531212</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>5670.06523480234</c:v>
+                  <c:v>11106.456705773</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4813.17055031031</c:v>
+                  <c:v>9865.33326709989</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>4934.14433712407</c:v>
+                  <c:v>9965.54516286339</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>5849.74321479961</c:v>
+                  <c:v>12017.0422206078</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>4939.50789450356</c:v>
+                  <c:v>9951.55030714782</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>4980.94494219129</c:v>
+                  <c:v>9942.51339700484</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>5863.76091420134</c:v>
+                  <c:v>12021.0304119956</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>5026.2282161644</c:v>
+                  <c:v>10948.7406469278</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>4830.78975293069</c:v>
+                  <c:v>10561.9297905285</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>5628.55674241922</c:v>
+                  <c:v>12901.141297832</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4794.88468246875</c:v>
+                  <c:v>10019.1353499615</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4768.27644620319</c:v>
+                  <c:v>9923.50106257438</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>5768.61738805403</c:v>
+                  <c:v>12184.0856379776</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>4827.1597067861</c:v>
+                  <c:v>10122.6218552879</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>4769.94279271094</c:v>
+                  <c:v>9974.50118387367</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>5761.3516367361</c:v>
+                  <c:v>12254.6820737545</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>4936.60182416066</c:v>
+                  <c:v>9625.86792014302</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>4858.45880112004</c:v>
+                  <c:v>9608.76030809579</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>5753.05369069636</c:v>
+                  <c:v>11727.9092571644</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>4892.11105453774</c:v>
+                  <c:v>10382.0670660383</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>4662.23988657354</c:v>
+                  <c:v>10089.5105904896</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>5593.12288693434</c:v>
+                  <c:v>12488.1663153958</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>4672.79947170339</c:v>
+                  <c:v>9480.475666447101</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>4545.56093023288</c:v>
+                  <c:v>9232.61313673986</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>5616.89308773079</c:v>
+                  <c:v>11561.3946389896</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>4680.97836465979</c:v>
+                  <c:v>8727.28129529874</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>4511.15613681332</c:v>
+                  <c:v>8357.94000223804</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3422,11 +3416,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2120911576"/>
-        <c:axId val="2115422152"/>
+        <c:axId val="-2141059992"/>
+        <c:axId val="-2141057048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2120911576"/>
+        <c:axId val="-2141059992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3435,7 +3429,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115422152"/>
+        <c:crossAx val="-2141057048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3443,7 +3437,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115422152"/>
+        <c:axId val="-2141057048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3454,7 +3448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120911576"/>
+        <c:crossAx val="-2141059992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17461,15 +17455,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:D83"/>
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1">
         <v>0</v>
       </c>
@@ -17477,10 +17471,13 @@
         <v>32213</v>
       </c>
       <c r="C1">
-        <v>3725.8831490019702</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>2471.9080171619698</v>
+      </c>
+      <c r="D1">
+        <v>10.220000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -17488,10 +17485,13 @@
         <v>64432</v>
       </c>
       <c r="C2">
-        <v>3725.8925012085201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>2471.9076142058302</v>
+      </c>
+      <c r="D2">
+        <v>10.220000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -17499,10 +17499,13 @@
         <v>101413</v>
       </c>
       <c r="C3">
-        <v>4400.7193963104601</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>2832.1053476379602</v>
+      </c>
+      <c r="D3">
+        <v>10.220000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -17510,10 +17513,13 @@
         <v>134305</v>
       </c>
       <c r="C4">
-        <v>4041.85111196139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>2946.31433087394</v>
+      </c>
+      <c r="D4">
+        <v>12.18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -17521,10 +17527,13 @@
         <v>166721</v>
       </c>
       <c r="C5">
-        <v>3977.0175328174701</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>2937.6615026519898</v>
+      </c>
+      <c r="D5">
+        <v>12.18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -17532,10 +17541,13 @@
         <v>199691</v>
       </c>
       <c r="C6">
-        <v>4198.1610836707596</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>2988.00728319054</v>
+      </c>
+      <c r="D6">
+        <v>12.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -17543,10 +17555,13 @@
         <v>232713</v>
       </c>
       <c r="C7">
-        <v>4214.7254211855197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>2592.0510882168301</v>
+      </c>
+      <c r="D7">
+        <v>10.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -17554,10 +17569,13 @@
         <v>265616</v>
       </c>
       <c r="C8">
-        <v>4144.0115825141102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>2583.54032601889</v>
+      </c>
+      <c r="D8">
+        <v>10.45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -17565,10 +17583,13 @@
         <v>303948</v>
       </c>
       <c r="C9">
-        <v>4797.1746000753601</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>2992.1160854505201</v>
+      </c>
+      <c r="D9">
+        <v>10.45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -17576,10 +17597,13 @@
         <v>337692</v>
       </c>
       <c r="C10">
-        <v>4258.3197548051703</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>3458.5313264306001</v>
+      </c>
+      <c r="D10">
+        <v>13.62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -17587,10 +17611,13 @@
         <v>371144</v>
       </c>
       <c r="C11">
-        <v>4214.0512640720199</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>3447.3348870449099</v>
+      </c>
+      <c r="D11">
+        <v>13.62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -17598,10 +17625,13 @@
         <v>405147</v>
       </c>
       <c r="C12">
-        <v>4309.3284046932004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>3502.6227861530801</v>
+      </c>
+      <c r="D12">
+        <v>13.62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -17609,10 +17639,13 @@
         <v>439074</v>
       </c>
       <c r="C13">
-        <v>4284.3987866470497</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>4550.8508060548802</v>
+      </c>
+      <c r="D13">
+        <v>17.57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -17620,10 +17653,13 @@
         <v>472817</v>
       </c>
       <c r="C14">
-        <v>4255.2313126610197</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>4530.8819630333201</v>
+      </c>
+      <c r="D14">
+        <v>17.57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -17631,10 +17667,13 @@
         <v>512474</v>
       </c>
       <c r="C15">
-        <v>4988.9613009483301</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>5335.5759672632003</v>
+      </c>
+      <c r="D15">
+        <v>17.57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -17642,10 +17681,13 @@
         <v>546797</v>
       </c>
       <c r="C16">
-        <v>4363.8766039226202</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>5721.0516006324697</v>
+      </c>
+      <c r="D16">
+        <v>21.74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -17653,10 +17695,13 @@
         <v>580400</v>
       </c>
       <c r="C17">
-        <v>4250.7613341605502</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>5604.3967198042801</v>
+      </c>
+      <c r="D17">
+        <v>21.74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -17664,10 +17709,13 @@
         <v>614822</v>
       </c>
       <c r="C18">
-        <v>4323.9919779121701</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>5734.8575449485397</v>
+      </c>
+      <c r="D18">
+        <v>21.74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -17675,10 +17723,13 @@
         <v>648968</v>
       </c>
       <c r="C19">
-        <v>4336.7440617718503</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>6539.6666470482796</v>
+      </c>
+      <c r="D19">
+        <v>24.98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -17686,10 +17737,13 @@
         <v>683003</v>
       </c>
       <c r="C20">
-        <v>4281.1437077166102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>6540.2318357846698</v>
+      </c>
+      <c r="D20">
+        <v>24.98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -17697,10 +17751,13 @@
         <v>723429</v>
       </c>
       <c r="C21">
-        <v>5040.03396070909</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>7765.9078526166404</v>
+      </c>
+      <c r="D21">
+        <v>24.98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
@@ -17708,10 +17765,13 @@
         <v>757911</v>
       </c>
       <c r="C22">
-        <v>4323.90265980392</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>6537.4423317577302</v>
+      </c>
+      <c r="D22">
+        <v>24.72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
@@ -17719,10 +17779,13 @@
         <v>792391</v>
       </c>
       <c r="C23">
-        <v>4345.3509790900498</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>6530.8947343809996</v>
+      </c>
+      <c r="D23">
+        <v>24.72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -17730,10 +17793,13 @@
         <v>827569</v>
       </c>
       <c r="C24">
-        <v>4416.9764845952604</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>6657.7235558374896</v>
+      </c>
+      <c r="D24">
+        <v>24.72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -17741,10 +17807,13 @@
         <v>862214</v>
       </c>
       <c r="C25">
-        <v>4395.1099991506198</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>7248.2531502322499</v>
+      </c>
+      <c r="D25">
+        <v>27.47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -17752,10 +17821,13 @@
         <v>896781</v>
       </c>
       <c r="C26">
-        <v>4382.5392071578899</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>7215.3646584775097</v>
+      </c>
+      <c r="D26">
+        <v>27.47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -17763,10 +17835,13 @@
         <v>938234</v>
       </c>
       <c r="C27">
-        <v>5124.2921033625698</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>8457.8822892203607</v>
+      </c>
+      <c r="D27">
+        <v>27.47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -17774,10 +17849,13 @@
         <v>973456</v>
       </c>
       <c r="C28">
-        <v>4896.2341075664699</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>8119.6228014705903</v>
+      </c>
+      <c r="D28">
+        <v>30.64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
@@ -17785,10 +17863,13 @@
         <v>1008067</v>
       </c>
       <c r="C29">
-        <v>4659.66430010356</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>8159.0324143647003</v>
+      </c>
+      <c r="D29">
+        <v>30.64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>29</v>
       </c>
@@ -17796,10 +17877,13 @@
         <v>1043694</v>
       </c>
       <c r="C30">
-        <v>4773.1778994218603</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>8371.5689930035605</v>
+      </c>
+      <c r="D30">
+        <v>30.64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>30</v>
       </c>
@@ -17807,10 +17891,13 @@
         <v>1078847</v>
       </c>
       <c r="C31">
-        <v>4639.2504806706902</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>6568.3226521368297</v>
+      </c>
+      <c r="D31">
+        <v>24.46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -17818,10 +17905,13 @@
         <v>1113885</v>
       </c>
       <c r="C32">
-        <v>4648.6781772282102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>6522.3307354685503</v>
+      </c>
+      <c r="D32">
+        <v>24.46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>32</v>
       </c>
@@ -17829,10 +17919,13 @@
         <v>1156130</v>
       </c>
       <c r="C33">
-        <v>5524.30218376842</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>7851.9304675793101</v>
+      </c>
+      <c r="D33">
+        <v>24.46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>33</v>
       </c>
@@ -17840,10 +17933,13 @@
         <v>1191777</v>
       </c>
       <c r="C34">
-        <v>4714.0227106090797</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>7523.3521671827302</v>
+      </c>
+      <c r="D34">
+        <v>27.79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>34</v>
       </c>
@@ -17851,10 +17947,13 @@
         <v>1227140</v>
       </c>
       <c r="C35">
-        <v>4693.6667377521298</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>7453.3679762620204</v>
+      </c>
+      <c r="D35">
+        <v>27.79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>35</v>
       </c>
@@ -17862,10 +17961,13 @@
         <v>1263685</v>
       </c>
       <c r="C36">
-        <v>4898.9558104895304</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>7696.2380002729296</v>
+      </c>
+      <c r="D36">
+        <v>27.79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>36</v>
       </c>
@@ -17873,10 +17975,13 @@
         <v>1299258</v>
       </c>
       <c r="C37">
-        <v>4778.2794463369801</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>7919.2885658806399</v>
+      </c>
+      <c r="D37">
+        <v>29.43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>37</v>
       </c>
@@ -17884,10 +17989,13 @@
         <v>1334967</v>
       </c>
       <c r="C38">
-        <v>4782.6163219314203</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>7954.1561230329698</v>
+      </c>
+      <c r="D38">
+        <v>29.43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>38</v>
       </c>
@@ -17895,10 +18003,13 @@
         <v>1377770</v>
       </c>
       <c r="C39">
-        <v>5644.8394989436101</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>9507.9891287636092</v>
+      </c>
+      <c r="D39">
+        <v>29.43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>39</v>
       </c>
@@ -17906,10 +18017,13 @@
         <v>1413671</v>
       </c>
       <c r="C40">
-        <v>4826.6168703633602</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>7446.6462015152301</v>
+      </c>
+      <c r="D40">
+        <v>27.49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>40</v>
       </c>
@@ -17917,10 +18031,13 @@
         <v>1449780</v>
       </c>
       <c r="C41">
-        <v>4778.3941670525301</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>7477.3399240877798</v>
+      </c>
+      <c r="D41">
+        <v>27.49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>41</v>
       </c>
@@ -17928,10 +18045,13 @@
         <v>1486647</v>
       </c>
       <c r="C42">
-        <v>4820.7184267789698</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>7613.0337348584499</v>
+      </c>
+      <c r="D42">
+        <v>27.49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>42</v>
       </c>
@@ -17939,10 +18059,13 @@
         <v>1522617</v>
       </c>
       <c r="C43">
-        <v>4734.3769846948999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>7323.1712127580204</v>
+      </c>
+      <c r="D43">
+        <v>27.09</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>43</v>
       </c>
@@ -17950,10 +18073,13 @@
         <v>1558893</v>
       </c>
       <c r="C44">
-        <v>4706.7448758225</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>7386.9806670028702</v>
+      </c>
+      <c r="D44">
+        <v>27.09</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>44</v>
       </c>
@@ -17961,10 +18087,13 @@
         <v>1602586</v>
       </c>
       <c r="C45">
-        <v>5619.79781996368</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>8882.2789876360002</v>
+      </c>
+      <c r="D45">
+        <v>27.09</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>45</v>
       </c>
@@ -17972,10 +18101,13 @@
         <v>1639346</v>
       </c>
       <c r="C46">
-        <v>4819.2510926942005</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>8826.4678066173092</v>
+      </c>
+      <c r="D46">
+        <v>32.04</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>46</v>
       </c>
@@ -17983,10 +18115,13 @@
         <v>1675783</v>
       </c>
       <c r="C47">
-        <v>4784.2129364080802</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>8745.9253896323808</v>
+      </c>
+      <c r="D47">
+        <v>32.04</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>47</v>
       </c>
@@ -17994,10 +18129,13 @@
         <v>1719640</v>
       </c>
       <c r="C48">
-        <v>5644.30603176369</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>10505.3051095258</v>
+      </c>
+      <c r="D48">
+        <v>32.04</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>48</v>
       </c>
@@ -18005,10 +18143,13 @@
         <v>1756071</v>
       </c>
       <c r="C49">
-        <v>4794.48243949468</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>9595.5228511567693</v>
+      </c>
+      <c r="D49">
+        <v>35.29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>49</v>
       </c>
@@ -18016,10 +18157,13 @@
         <v>1792510</v>
       </c>
       <c r="C50">
-        <v>4798.9647724514998</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>9663.36865260388</v>
+      </c>
+      <c r="D50">
+        <v>35.29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>50</v>
       </c>
@@ -18027,10 +18171,13 @@
         <v>1836336</v>
       </c>
       <c r="C51">
-        <v>5658.5114680775996</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>11627.720070580301</v>
+      </c>
+      <c r="D51">
+        <v>35.29</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>51</v>
       </c>
@@ -18038,10 +18185,13 @@
         <v>1873185</v>
       </c>
       <c r="C52">
-        <v>4852.7354030103197</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+        <v>9832.0455397051992</v>
+      </c>
+      <c r="D52">
+        <v>35.57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>52</v>
       </c>
@@ -18049,10 +18199,13 @@
         <v>1909427</v>
       </c>
       <c r="C53">
-        <v>4707.2292269301097</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+        <v>9654.4233798374098</v>
+      </c>
+      <c r="D53">
+        <v>35.57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>53</v>
       </c>
@@ -18060,10 +18213,13 @@
         <v>1953594</v>
       </c>
       <c r="C54">
-        <v>5591.2392696529396</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+        <v>11724.8489980831</v>
+      </c>
+      <c r="D54">
+        <v>35.57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>54</v>
       </c>
@@ -18071,10 +18227,13 @@
         <v>1990891</v>
       </c>
       <c r="C55">
-        <v>4779.4948971601898</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>9236.1652686305497</v>
+      </c>
+      <c r="D55">
+        <v>33.21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>55</v>
       </c>
@@ -18082,10 +18241,13 @@
         <v>2027999</v>
       </c>
       <c r="C56">
-        <v>4743.9727216765596</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>9196.73381531212</v>
+      </c>
+      <c r="D56">
+        <v>33.21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>56</v>
       </c>
@@ -18093,10 +18255,13 @@
         <v>2072999</v>
       </c>
       <c r="C57">
-        <v>5670.0652348023395</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>11106.456705773</v>
+      </c>
+      <c r="D57">
+        <v>33.21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>57</v>
       </c>
@@ -18104,10 +18269,13 @@
         <v>2110677</v>
       </c>
       <c r="C58">
-        <v>4813.1705503103103</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>9865.3332670998898</v>
+      </c>
+      <c r="D58">
+        <v>35.28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>58</v>
       </c>
@@ -18115,10 +18283,13 @@
         <v>2148707</v>
       </c>
       <c r="C59">
-        <v>4934.1443371240703</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+        <v>9965.5451628633891</v>
+      </c>
+      <c r="D59">
+        <v>35.28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>59</v>
       </c>
@@ -18126,10 +18297,13 @@
         <v>2194551</v>
       </c>
       <c r="C60">
-        <v>5849.7432147996096</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>12017.0422206078</v>
+      </c>
+      <c r="D60">
+        <v>35.28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61">
         <v>60</v>
       </c>
@@ -18137,10 +18311,13 @@
         <v>2232523</v>
       </c>
       <c r="C61">
-        <v>4939.5078945035602</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>9951.5503071478197</v>
+      </c>
+      <c r="D61">
+        <v>35.32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62">
         <v>61</v>
       </c>
@@ -18148,10 +18325,13 @@
         <v>2270520</v>
       </c>
       <c r="C62">
-        <v>4980.9449421912896</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+        <v>9942.5133970048391</v>
+      </c>
+      <c r="D62">
+        <v>35.32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63">
         <v>62</v>
       </c>
@@ -18159,10 +18339,13 @@
         <v>2316439</v>
       </c>
       <c r="C63">
-        <v>5863.7609142013398</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+        <v>12021.0304119956</v>
+      </c>
+      <c r="D63">
+        <v>35.32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>63</v>
       </c>
@@ -18170,10 +18353,13 @@
         <v>2354948</v>
       </c>
       <c r="C64">
-        <v>5026.2282161643998</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+        <v>10948.740646927799</v>
+      </c>
+      <c r="D64">
+        <v>38.44</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>64</v>
       </c>
@@ -18181,10 +18367,13 @@
         <v>2392206</v>
       </c>
       <c r="C65">
-        <v>4830.7897529306902</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+        <v>10561.9297905285</v>
+      </c>
+      <c r="D65">
+        <v>38.44</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66">
         <v>65</v>
       </c>
@@ -18192,10 +18381,13 @@
         <v>2437835</v>
       </c>
       <c r="C66">
-        <v>5628.5567424192204</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+        <v>12901.141297832</v>
+      </c>
+      <c r="D66">
+        <v>38.44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67">
         <v>66</v>
       </c>
@@ -18203,10 +18395,13 @@
         <v>2475227</v>
       </c>
       <c r="C67">
-        <v>4794.8846824687498</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+        <v>10019.1353499615</v>
+      </c>
+      <c r="D67">
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68">
         <v>67</v>
       </c>
@@ -18214,10 +18409,13 @@
         <v>2512326</v>
       </c>
       <c r="C68">
-        <v>4768.2764462031901</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+        <v>9923.5010625743798</v>
+      </c>
+      <c r="D68">
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69">
         <v>68</v>
       </c>
@@ -18225,10 +18423,13 @@
         <v>2557838</v>
       </c>
       <c r="C69">
-        <v>5768.61738805403</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+        <v>12184.0856379776</v>
+      </c>
+      <c r="D69">
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70">
         <v>69</v>
       </c>
@@ -18236,10 +18437,13 @@
         <v>2595225</v>
       </c>
       <c r="C70">
-        <v>4827.1597067861003</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+        <v>10122.6218552879</v>
+      </c>
+      <c r="D70">
+        <v>37.11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71">
         <v>70</v>
       </c>
@@ -18247,10 +18451,13 @@
         <v>2632082</v>
       </c>
       <c r="C71">
-        <v>4769.94279271094</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
+        <v>9974.50118387367</v>
+      </c>
+      <c r="D71">
+        <v>37.11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72">
         <v>71</v>
       </c>
@@ -18258,10 +18465,13 @@
         <v>2677387</v>
       </c>
       <c r="C72">
-        <v>5761.3516367360999</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+        <v>12254.6820737545</v>
+      </c>
+      <c r="D72">
+        <v>37.11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73">
         <v>72</v>
       </c>
@@ -18269,10 +18479,13 @@
         <v>2714383</v>
       </c>
       <c r="C73">
-        <v>4936.6018241606598</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
+        <v>9625.8679201430205</v>
+      </c>
+      <c r="D73">
+        <v>35.74</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74">
         <v>73</v>
       </c>
@@ -18280,10 +18493,13 @@
         <v>2751229</v>
       </c>
       <c r="C74">
-        <v>4858.4588011200403</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
+        <v>9608.7603080957906</v>
+      </c>
+      <c r="D74">
+        <v>35.74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75">
         <v>74</v>
       </c>
@@ -18291,10 +18507,13 @@
         <v>2796295</v>
       </c>
       <c r="C75">
-        <v>5753.0536906963598</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
+        <v>11727.9092571644</v>
+      </c>
+      <c r="D75">
+        <v>35.74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76">
         <v>75</v>
       </c>
@@ -18302,10 +18521,13 @@
         <v>2833135</v>
       </c>
       <c r="C76">
-        <v>4892.1110545377396</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
+        <v>10382.0670660383</v>
+      </c>
+      <c r="D76">
+        <v>38.770000000000003</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77">
         <v>76</v>
       </c>
@@ -18313,10 +18535,13 @@
         <v>2868968</v>
       </c>
       <c r="C77">
-        <v>4662.2398865735404</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
+        <v>10089.510590489601</v>
+      </c>
+      <c r="D77">
+        <v>38.770000000000003</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78">
         <v>77</v>
       </c>
@@ -18324,10 +18549,13 @@
         <v>2913441</v>
       </c>
       <c r="C78">
-        <v>5593.1228869343404</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
+        <v>12488.1663153958</v>
+      </c>
+      <c r="D78">
+        <v>38.770000000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79">
         <v>78</v>
       </c>
@@ -18335,10 +18563,13 @@
         <v>2949459</v>
       </c>
       <c r="C79">
-        <v>4672.7994717033898</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
+        <v>9480.4756664471006</v>
+      </c>
+      <c r="D79">
+        <v>36.25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80">
         <v>79</v>
       </c>
@@ -18346,10 +18577,13 @@
         <v>2984633</v>
       </c>
       <c r="C80">
-        <v>4545.5609302328803</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
+        <v>9232.6131367398593</v>
+      </c>
+      <c r="D80">
+        <v>36.25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81">
         <v>80</v>
       </c>
@@ -18357,10 +18591,13 @@
         <v>3028639</v>
       </c>
       <c r="C81">
-        <v>5616.8930877307903</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
+        <v>11561.394638989599</v>
+      </c>
+      <c r="D81">
+        <v>36.25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82">
         <v>81</v>
       </c>
@@ -18368,10 +18605,13 @@
         <v>3064728</v>
       </c>
       <c r="C82">
-        <v>4680.9783646597898</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
+        <v>8727.2812952987406</v>
+      </c>
+      <c r="D82">
+        <v>33.35</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83">
         <v>82</v>
       </c>
@@ -18379,7 +18619,10 @@
         <v>3099285</v>
       </c>
       <c r="C83">
-        <v>4511.1561368133198</v>
+        <v>8357.9400022380396</v>
+      </c>
+      <c r="D83">
+        <v>33.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update - new experiments
</commit_message>
<xml_diff>
--- a/extensions/ida2016/doc-Experiments/ExperimentsResults.xlsx
+++ b/extensions/ida2016/doc-Experiments/ExperimentsResults.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22500" tabRatio="500" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="13920" tabRatio="500" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
-    <sheet name="ida2015" sheetId="1" r:id="rId1"/>
-    <sheet name="IDA2015Graph" sheetId="5" r:id="rId2"/>
+    <sheet name="IDA2015Graph" sheetId="5" r:id="rId1"/>
+    <sheet name="ida2015" sheetId="1" r:id="rId2"/>
     <sheet name="IDA2016NoBumps" sheetId="11" r:id="rId3"/>
     <sheet name="ida2016" sheetId="2" r:id="rId4"/>
     <sheet name="IDA2016Graph" sheetId="4" r:id="rId5"/>
@@ -18,6 +18,7 @@
     <sheet name="URGraphNoBumps" sheetId="10" r:id="rId9"/>
     <sheet name="URGraphNoBumpsUR" sheetId="12" r:id="rId10"/>
     <sheet name="withUnemplRateObserved" sheetId="7" r:id="rId11"/>
+    <sheet name="noResiduals" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="149">
   <si>
     <t>Sample</t>
   </si>
@@ -462,6 +463,21 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>UR original</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>UR zero</t>
+  </si>
+  <si>
+    <t>No UR var - seed 1</t>
+  </si>
+  <si>
+    <t>No UR var - seed 154</t>
+  </si>
 </sst>
 </file>
 
@@ -509,7 +525,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -525,12 +541,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -538,6 +565,10 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -545,6 +576,10 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -580,10 +615,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'ida2015'!$C$2:$C$43</c:f>
+              <c:f>'ida2015'!$D$48:$D$131</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="84"/>
                 <c:pt idx="0">
                   <c:v>2372.41437172793</c:v>
                 </c:pt>
@@ -709,6 +744,132 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>4810.66564528312</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4691.90732729206</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4725.66033890325</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5680.28653309161</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4808.84060341374</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4768.38312974166</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5716.24394001021</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4783.61194089902</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4789.42667298383</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5733.34608801486</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4848.49253433322</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4761.53321271724</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5745.60827254274</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4870.67844786203</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4855.0890254204</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5851.77936182761</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4930.35064407189</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4985.05600989755</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5985.84478664743</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4991.22394189275</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5009.42805219768</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6018.00208100256</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5087.76672413486</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4910.42711337323</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5902.86164950349</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4871.54042854612</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4861.1023329455</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>5945.83806578787</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4917.18681931747</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4858.48188160274</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5940.96689837518</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4901.4146027018</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4897.24886840752</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5917.61210034282</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4910.7388096513</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4746.98641104891</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>5811.21093089624</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4768.28830734431</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4643.15565931788</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>5783.48210729794</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4773.11071033681</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4590.8106327454</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>5766.57037773593</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -725,11 +886,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2141073096"/>
-        <c:axId val="-2120873816"/>
+        <c:axId val="-2122064472"/>
+        <c:axId val="-2122061528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2141073096"/>
+        <c:axId val="-2122064472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -738,7 +899,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120873816"/>
+        <c:crossAx val="-2122061528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -746,7 +907,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2120873816"/>
+        <c:axId val="-2122061528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -757,24 +918,20 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141073096"/>
+        <c:crossAx val="-2122064472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -3557,7 +3714,1001 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>noResiduals!$I$3:$I$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="63"/>
+                <c:pt idx="0">
+                  <c:v>3655.48961692169</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7299.65794880437</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11023.8296724436</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15590.4176307804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20393.2482388761</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25088.3343540118</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29644.520641206</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34401.523241736</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39392.1264750303</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44640.7220960009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50173.7969460629</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56140.0825276481</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>62672.7200182283</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>69694.59619032381</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>77375.9868110658</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85479.3215414509</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>94149.6969344738</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>103371.230296315</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>112936.277795864</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>123041.536745817</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>133363.593768741</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>144011.26597616</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>155276.685528819</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>166870.309919621</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>179176.186784912</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>191571.568865408</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>204018.373159349</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>216780.492511437</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>229701.90762747</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>243201.139246673</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>256572.197750719</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>270194.381728717</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>284055.483500343</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>298102.295816964</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>312586.156601997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>326844.981591253</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>341309.934145802</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>356182.724094808</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>371152.731606287</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>386402.099061719</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>401884.030410938</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>417811.432681419</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>433662.252598289</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>450174.20068718</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>466749.447027765</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>483775.523988675</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>501150.31949683</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>518758.513559161</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>536550.093829521</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>554784.947514632</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>572684.965078081</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>590751.4777421691</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>608864.170208898</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>627285.624571479</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>645618.389969809</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>664133.529067009</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>682712.743874294</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>701487.365252029</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>719868.191784187</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>738462.559882911</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>756732.954551847</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>775562.21784167</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>793621.554717963</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2101170408"/>
+        <c:axId val="2115908728"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2101170408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2115908728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2115908728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2101170408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>noResiduals!$G$3:$G$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="63"/>
+                <c:pt idx="0">
+                  <c:v>3695.65132983285</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7379.84612651819</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11142.994941302</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13547.2581641846</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15858.520211014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18377.3248910315</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21132.2070992059</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23827.3429242075</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26123.2362383636</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28205.7516041079</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29852.5426205378</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30945.2138369167</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>31460.0697056162</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>31359.9526102586</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30776.0138039851</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29687.3324960343</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28122.3531570251</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26185.7662066853</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23967.1083298451</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21396.6785568134</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>18604.8439093822</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15480.8911458694</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11830.623279647</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7691.65098294005</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2902.30804194928</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-2298.38644295423</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-7994.37098119328</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-14708.9474599311</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-22473.3556514982</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-31585.831248772</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-41816.1697167704</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-53479.9155247068</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-66536.8940010074</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-80909.4772822588</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-96614.0621670796</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-112894.463594978</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-129707.855665275</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-147000.746237521</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-164469.85029438</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-181981.945784843</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-199543.259396832</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-217227.851626102</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-234600.315874341</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-252275.583212695</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-269658.994280381</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-287194.411088043</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-304904.036796636</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-322630.485946057</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-340398.622123436</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-358498.419616957</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-376311.716799177</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-394228.979054141</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-412082.604446444</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-430173.945448887</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2102464776"/>
+        <c:axId val="-2144678360"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2102464776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2144678360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2144678360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2102464776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>noResiduals!$N$3:$N$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="63"/>
+                <c:pt idx="0">
+                  <c:v>3695.65132983285</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7379.84612651819</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11142.994941302</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13547.2581641846</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15858.520211014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18377.3248910315</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21132.2070992059</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23827.3429242075</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26123.2362383636</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28205.7516041079</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29852.5426205378</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30945.2138369167</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>31460.0697056162</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>31359.9526102586</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30776.0138039851</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29687.3324960343</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28122.3531570251</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26185.7662066853</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23967.1083298451</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21396.6785568134</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>18604.8439093822</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15480.8911458694</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11830.623279647</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7691.65098294005</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2902.30804194928</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-2298.38644295423</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-7994.37098119328</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-14708.9474599311</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-22473.3556514982</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-31585.831248772</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-41816.1697167704</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-53479.9155247068</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-66536.8940010074</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-80909.4772822588</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-96614.0621670796</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-112894.463594978</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-129707.855665275</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-147000.746237521</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2078171912"/>
+        <c:axId val="-2077043160"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2078171912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2077043160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2077043160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2078171912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'ida2015'!$C$2:$C$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>2372.41437172793</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1615.20571963503</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3392.16502769283</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3703.13859855302</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3828.81946685368</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3988.40375315707</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4082.96829283384</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4126.97961822896</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4846.38064812796</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4294.11206860795</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4269.43727801853</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4356.16718919735</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4350.87836841498</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4330.59438116778</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5092.27773955047</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4412.83317839302</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4327.62771125282</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4432.9145428868</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4402.6298572019</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4385.84779826794</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5207.65603655651</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4448.74855522494</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4455.72624755461</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4562.96828452503</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4485.08473847178</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4489.97157036886</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5347.80935983648</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4577.23289785248</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4503.99639598618</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4628.54806350651</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4566.91538029693</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4544.76243004434</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5473.46577182584</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4634.34932840615</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4604.50349767024</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4772.79076101849</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4652.68327596632</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4685.11858601232</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5586.02715075624</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4714.92579379838</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4728.90919254984</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4810.66564528312</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2141073096"/>
+        <c:axId val="-2120873816"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2141073096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2120873816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2120873816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2141073096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3906,354 +5057,6 @@
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'ida2015'!$D$48:$D$131</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="84"/>
-                <c:pt idx="0">
-                  <c:v>2372.41437172793</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1615.20571963503</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3392.16502769283</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3703.13859855302</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3828.81946685368</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3988.40375315707</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4082.96829283384</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4126.97961822896</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4846.38064812796</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4294.11206860795</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4269.43727801853</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4356.16718919735</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4350.87836841498</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4330.59438116778</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5092.27773955047</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4412.83317839302</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4327.62771125282</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4432.9145428868</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4402.6298572019</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4385.84779826794</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>5207.65603655651</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4448.74855522494</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4455.72624755461</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>4562.96828452503</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>4485.08473847178</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>4489.97157036886</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>5347.80935983648</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4577.23289785248</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>4503.99639598618</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>4628.54806350651</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>4566.91538029693</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>4544.76243004434</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>5473.46577182584</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>4634.34932840615</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>4604.50349767024</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>4772.79076101849</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>4652.68327596632</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>4685.11858601232</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>5586.02715075624</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>4714.92579379838</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>4728.90919254984</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>4810.66564528312</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>4691.90732729206</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>4725.66033890325</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>5680.28653309161</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>4808.84060341374</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>4768.38312974166</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>5716.24394001021</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>4783.61194089902</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>4789.42667298383</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>5733.34608801486</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>4848.49253433322</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>4761.53321271724</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5745.60827254274</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>4870.67844786203</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>4855.0890254204</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5851.77936182761</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>4930.35064407189</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>4985.05600989755</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5985.84478664743</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>4991.22394189275</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>5009.42805219768</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>6018.00208100256</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>5087.76672413486</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>4910.42711337323</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>5902.86164950349</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>4871.54042854612</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>4861.1023329455</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>5945.83806578787</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>4917.18681931747</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>4858.48188160274</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>5940.96689837518</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>4901.4146027018</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>4897.24886840752</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>5917.61210034282</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>4910.7388096513</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>4746.98641104891</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>5811.21093089624</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>4768.28830734431</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>4643.15565931788</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>5783.48210729794</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>4773.11071033681</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>4590.8106327454</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>5766.57037773593</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="-2122064472"/>
-        <c:axId val="-2122061528"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="-2122064472"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122061528"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-2122061528"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122064472"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
 </c:chartSpace>
 </file>
 
@@ -6369,7 +7172,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -6380,7 +7183,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6392,7 +7195,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -6415,7 +7218,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6427,7 +7230,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6439,7 +7242,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="204" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -6448,23 +7251,15 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9210081" cy="5616911"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6477,37 +7272,7 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 10"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6572,15 +7337,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6602,16 +7367,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6633,17 +7398,25 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9210081" cy="5616911"/>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6656,7 +7429,132 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:absoluteAnchor>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -21351,8 +22249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -24787,4 +25685,1311 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F1:N65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F36" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:N65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="6:14">
+      <c r="F1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="6:14">
+      <c r="F2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>145</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>145</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="6:14">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>3695.65132983285</v>
+      </c>
+      <c r="I3">
+        <v>3655.48961692169</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>3655.48961692169</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>3695.65132983285</v>
+      </c>
+    </row>
+    <row r="4" spans="6:14">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>7379.8461265181904</v>
+      </c>
+      <c r="I4">
+        <v>7299.6579488043699</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>7299.6579488043699</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>7379.8461265181904</v>
+      </c>
+    </row>
+    <row r="5" spans="6:14">
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>11142.994941302</v>
+      </c>
+      <c r="I5">
+        <v>11023.8296724436</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>11023.8296724436</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>11142.994941302</v>
+      </c>
+    </row>
+    <row r="6" spans="6:14">
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>13547.258164184601</v>
+      </c>
+      <c r="I6">
+        <v>15590.417630780399</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>15590.417630780399</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>13547.258164184601</v>
+      </c>
+    </row>
+    <row r="7" spans="6:14">
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>15858.520211014</v>
+      </c>
+      <c r="I7">
+        <v>20393.248238876098</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>20393.248238876</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>15858.520211014</v>
+      </c>
+    </row>
+    <row r="8" spans="6:14">
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>18377.324891031501</v>
+      </c>
+      <c r="I8">
+        <v>25088.3343540118</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>25088.334354011698</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8">
+        <v>18377.324891031501</v>
+      </c>
+    </row>
+    <row r="9" spans="6:14">
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>21132.207099205902</v>
+      </c>
+      <c r="I9">
+        <v>29644.520641206</v>
+      </c>
+      <c r="J9">
+        <v>7</v>
+      </c>
+      <c r="K9">
+        <v>29644.520641205901</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9">
+        <v>21132.207099205902</v>
+      </c>
+    </row>
+    <row r="10" spans="6:14">
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>23827.3429242075</v>
+      </c>
+      <c r="I10">
+        <v>34401.523241736002</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <v>34401.5232417359</v>
+      </c>
+      <c r="M10">
+        <v>9</v>
+      </c>
+      <c r="N10">
+        <v>23827.3429242075</v>
+      </c>
+    </row>
+    <row r="11" spans="6:14">
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>26123.236238363599</v>
+      </c>
+      <c r="I11">
+        <v>39392.126475030302</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>39392.126475030302</v>
+      </c>
+      <c r="M11">
+        <v>10</v>
+      </c>
+      <c r="N11">
+        <v>26123.236238363599</v>
+      </c>
+    </row>
+    <row r="12" spans="6:14">
+      <c r="F12">
+        <v>11</v>
+      </c>
+      <c r="G12">
+        <v>28205.7516041079</v>
+      </c>
+      <c r="I12">
+        <v>44640.7220960009</v>
+      </c>
+      <c r="J12">
+        <v>11</v>
+      </c>
+      <c r="K12">
+        <v>44640.722096000798</v>
+      </c>
+      <c r="M12">
+        <v>11</v>
+      </c>
+      <c r="N12">
+        <v>28205.7516041079</v>
+      </c>
+    </row>
+    <row r="13" spans="6:14">
+      <c r="F13">
+        <v>12</v>
+      </c>
+      <c r="G13">
+        <v>29852.542620537799</v>
+      </c>
+      <c r="I13">
+        <v>50173.796946062903</v>
+      </c>
+      <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="K13">
+        <v>50173.796946062801</v>
+      </c>
+      <c r="M13">
+        <v>12</v>
+      </c>
+      <c r="N13">
+        <v>29852.542620537799</v>
+      </c>
+    </row>
+    <row r="14" spans="6:14">
+      <c r="F14">
+        <v>13</v>
+      </c>
+      <c r="G14">
+        <v>30945.213836916701</v>
+      </c>
+      <c r="I14">
+        <v>56140.082527648097</v>
+      </c>
+      <c r="J14">
+        <v>13</v>
+      </c>
+      <c r="K14">
+        <v>56140.082527648003</v>
+      </c>
+      <c r="M14">
+        <v>13</v>
+      </c>
+      <c r="N14">
+        <v>30945.213836916701</v>
+      </c>
+    </row>
+    <row r="15" spans="6:14">
+      <c r="F15">
+        <v>15</v>
+      </c>
+      <c r="G15">
+        <v>31460.069705616199</v>
+      </c>
+      <c r="I15">
+        <v>62672.720018228298</v>
+      </c>
+      <c r="J15">
+        <v>15</v>
+      </c>
+      <c r="K15">
+        <v>62672.720018228298</v>
+      </c>
+      <c r="M15">
+        <v>15</v>
+      </c>
+      <c r="N15">
+        <v>31460.069705616199</v>
+      </c>
+    </row>
+    <row r="16" spans="6:14">
+      <c r="F16">
+        <v>16</v>
+      </c>
+      <c r="G16">
+        <v>31359.952610258599</v>
+      </c>
+      <c r="I16">
+        <v>69694.596190323806</v>
+      </c>
+      <c r="J16">
+        <v>16</v>
+      </c>
+      <c r="K16">
+        <v>69694.596190323704</v>
+      </c>
+      <c r="M16">
+        <v>16</v>
+      </c>
+      <c r="N16">
+        <v>31359.952610258599</v>
+      </c>
+    </row>
+    <row r="17" spans="6:14">
+      <c r="F17">
+        <v>17</v>
+      </c>
+      <c r="G17">
+        <v>30776.013803985101</v>
+      </c>
+      <c r="I17">
+        <v>77375.986811065799</v>
+      </c>
+      <c r="J17">
+        <v>17</v>
+      </c>
+      <c r="K17">
+        <v>77375.986811065697</v>
+      </c>
+      <c r="M17">
+        <v>17</v>
+      </c>
+      <c r="N17">
+        <v>30776.013803985101</v>
+      </c>
+    </row>
+    <row r="18" spans="6:14">
+      <c r="F18">
+        <v>18</v>
+      </c>
+      <c r="G18">
+        <v>29687.332496034302</v>
+      </c>
+      <c r="I18">
+        <v>85479.321541450903</v>
+      </c>
+      <c r="J18">
+        <v>18</v>
+      </c>
+      <c r="K18">
+        <v>85479.321541450699</v>
+      </c>
+      <c r="M18">
+        <v>18</v>
+      </c>
+      <c r="N18">
+        <v>29687.332496034302</v>
+      </c>
+    </row>
+    <row r="19" spans="6:14">
+      <c r="F19">
+        <v>19</v>
+      </c>
+      <c r="G19">
+        <v>28122.3531570251</v>
+      </c>
+      <c r="I19">
+        <v>94149.696934473803</v>
+      </c>
+      <c r="J19">
+        <v>19</v>
+      </c>
+      <c r="K19">
+        <v>94149.696934473599</v>
+      </c>
+      <c r="M19">
+        <v>19</v>
+      </c>
+      <c r="N19">
+        <v>28122.3531570251</v>
+      </c>
+    </row>
+    <row r="20" spans="6:14">
+      <c r="F20">
+        <v>21</v>
+      </c>
+      <c r="G20">
+        <v>26185.766206685301</v>
+      </c>
+      <c r="I20">
+        <v>103371.230296315</v>
+      </c>
+      <c r="J20">
+        <v>21</v>
+      </c>
+      <c r="K20">
+        <v>103371.230296315</v>
+      </c>
+      <c r="M20">
+        <v>21</v>
+      </c>
+      <c r="N20">
+        <v>26185.766206685301</v>
+      </c>
+    </row>
+    <row r="21" spans="6:14">
+      <c r="F21">
+        <v>22</v>
+      </c>
+      <c r="G21">
+        <v>23967.108329845101</v>
+      </c>
+      <c r="I21">
+        <v>112936.27779586401</v>
+      </c>
+      <c r="J21">
+        <v>22</v>
+      </c>
+      <c r="K21">
+        <v>112936.27779586401</v>
+      </c>
+      <c r="M21">
+        <v>22</v>
+      </c>
+      <c r="N21">
+        <v>23967.108329845101</v>
+      </c>
+    </row>
+    <row r="22" spans="6:14">
+      <c r="F22">
+        <v>23</v>
+      </c>
+      <c r="G22">
+        <v>21396.6785568134</v>
+      </c>
+      <c r="I22">
+        <v>123041.53674581699</v>
+      </c>
+      <c r="J22">
+        <v>23</v>
+      </c>
+      <c r="K22">
+        <v>123041.53674581699</v>
+      </c>
+      <c r="M22">
+        <v>23</v>
+      </c>
+      <c r="N22">
+        <v>21396.6785568134</v>
+      </c>
+    </row>
+    <row r="23" spans="6:14">
+      <c r="F23">
+        <v>24</v>
+      </c>
+      <c r="G23">
+        <v>18604.843909382202</v>
+      </c>
+      <c r="I23">
+        <v>133363.593768741</v>
+      </c>
+      <c r="J23">
+        <v>24</v>
+      </c>
+      <c r="K23">
+        <v>133363.59376873999</v>
+      </c>
+      <c r="M23">
+        <v>24</v>
+      </c>
+      <c r="N23">
+        <v>18604.843909382202</v>
+      </c>
+    </row>
+    <row r="24" spans="6:14">
+      <c r="F24">
+        <v>25</v>
+      </c>
+      <c r="G24">
+        <v>15480.8911458694</v>
+      </c>
+      <c r="I24">
+        <v>144011.26597616001</v>
+      </c>
+      <c r="J24">
+        <v>25</v>
+      </c>
+      <c r="K24">
+        <v>144011.26597616001</v>
+      </c>
+      <c r="M24">
+        <v>25</v>
+      </c>
+      <c r="N24">
+        <v>15480.8911458694</v>
+      </c>
+    </row>
+    <row r="25" spans="6:14">
+      <c r="F25">
+        <v>27</v>
+      </c>
+      <c r="G25">
+        <v>11830.623279646999</v>
+      </c>
+      <c r="I25">
+        <v>155276.68552881901</v>
+      </c>
+      <c r="J25">
+        <v>27</v>
+      </c>
+      <c r="K25">
+        <v>155276.68552881799</v>
+      </c>
+      <c r="M25">
+        <v>27</v>
+      </c>
+      <c r="N25">
+        <v>11830.623279646999</v>
+      </c>
+    </row>
+    <row r="26" spans="6:14">
+      <c r="F26">
+        <v>28</v>
+      </c>
+      <c r="G26">
+        <v>7691.6509829400502</v>
+      </c>
+      <c r="I26">
+        <v>166870.30991962101</v>
+      </c>
+      <c r="J26">
+        <v>28</v>
+      </c>
+      <c r="K26">
+        <v>166870.30991962101</v>
+      </c>
+      <c r="M26">
+        <v>28</v>
+      </c>
+      <c r="N26">
+        <v>7691.6509829400502</v>
+      </c>
+    </row>
+    <row r="27" spans="6:14">
+      <c r="F27">
+        <v>29</v>
+      </c>
+      <c r="G27">
+        <v>2902.3080419492799</v>
+      </c>
+      <c r="I27">
+        <v>179176.18678491199</v>
+      </c>
+      <c r="J27">
+        <v>29</v>
+      </c>
+      <c r="K27">
+        <v>179176.18678491199</v>
+      </c>
+      <c r="M27">
+        <v>29</v>
+      </c>
+      <c r="N27">
+        <v>2902.3080419492799</v>
+      </c>
+    </row>
+    <row r="28" spans="6:14">
+      <c r="F28">
+        <v>30</v>
+      </c>
+      <c r="G28">
+        <v>-2298.38644295423</v>
+      </c>
+      <c r="I28">
+        <v>191571.56886540799</v>
+      </c>
+      <c r="J28">
+        <v>30</v>
+      </c>
+      <c r="K28">
+        <v>191571.56886540799</v>
+      </c>
+      <c r="M28">
+        <v>30</v>
+      </c>
+      <c r="N28">
+        <v>-2298.38644295423</v>
+      </c>
+    </row>
+    <row r="29" spans="6:14">
+      <c r="F29">
+        <v>31</v>
+      </c>
+      <c r="G29">
+        <v>-7994.3709811932804</v>
+      </c>
+      <c r="I29">
+        <v>204018.37315934899</v>
+      </c>
+      <c r="J29">
+        <v>31</v>
+      </c>
+      <c r="K29">
+        <v>204018.37315934899</v>
+      </c>
+      <c r="M29">
+        <v>31</v>
+      </c>
+      <c r="N29">
+        <v>-7994.3709811932804</v>
+      </c>
+    </row>
+    <row r="30" spans="6:14">
+      <c r="F30">
+        <v>33</v>
+      </c>
+      <c r="G30">
+        <v>-14708.9474599311</v>
+      </c>
+      <c r="I30">
+        <v>216780.49251143701</v>
+      </c>
+      <c r="J30">
+        <v>33</v>
+      </c>
+      <c r="K30">
+        <v>216780.49251143701</v>
+      </c>
+      <c r="M30">
+        <v>33</v>
+      </c>
+      <c r="N30">
+        <v>-14708.9474599311</v>
+      </c>
+    </row>
+    <row r="31" spans="6:14">
+      <c r="F31">
+        <v>34</v>
+      </c>
+      <c r="G31">
+        <v>-22473.355651498201</v>
+      </c>
+      <c r="I31">
+        <v>229701.90762747001</v>
+      </c>
+      <c r="J31">
+        <v>34</v>
+      </c>
+      <c r="K31">
+        <v>229701.90762747001</v>
+      </c>
+      <c r="M31">
+        <v>34</v>
+      </c>
+      <c r="N31">
+        <v>-22473.355651498201</v>
+      </c>
+    </row>
+    <row r="32" spans="6:14">
+      <c r="F32">
+        <v>35</v>
+      </c>
+      <c r="G32">
+        <v>-31585.831248772</v>
+      </c>
+      <c r="I32">
+        <v>243201.139246673</v>
+      </c>
+      <c r="J32">
+        <v>35</v>
+      </c>
+      <c r="K32">
+        <v>243201.139246673</v>
+      </c>
+      <c r="M32">
+        <v>35</v>
+      </c>
+      <c r="N32">
+        <v>-31585.831248772</v>
+      </c>
+    </row>
+    <row r="33" spans="6:14">
+      <c r="F33">
+        <v>36</v>
+      </c>
+      <c r="G33">
+        <v>-41816.169716770397</v>
+      </c>
+      <c r="I33">
+        <v>256572.197750719</v>
+      </c>
+      <c r="J33">
+        <v>36</v>
+      </c>
+      <c r="K33">
+        <v>256572.197750719</v>
+      </c>
+      <c r="M33">
+        <v>36</v>
+      </c>
+      <c r="N33">
+        <v>-41816.169716770397</v>
+      </c>
+    </row>
+    <row r="34" spans="6:14">
+      <c r="F34">
+        <v>37</v>
+      </c>
+      <c r="G34">
+        <v>-53479.915524706797</v>
+      </c>
+      <c r="I34">
+        <v>270194.38172871701</v>
+      </c>
+      <c r="J34">
+        <v>37</v>
+      </c>
+      <c r="K34">
+        <v>270194.38172871701</v>
+      </c>
+      <c r="M34">
+        <v>37</v>
+      </c>
+      <c r="N34">
+        <v>-53479.915524706797</v>
+      </c>
+    </row>
+    <row r="35" spans="6:14">
+      <c r="F35">
+        <v>39</v>
+      </c>
+      <c r="G35">
+        <v>-66536.8940010074</v>
+      </c>
+      <c r="I35">
+        <v>284055.48350034299</v>
+      </c>
+      <c r="J35">
+        <v>39</v>
+      </c>
+      <c r="K35">
+        <v>284055.48350034299</v>
+      </c>
+      <c r="M35">
+        <v>39</v>
+      </c>
+      <c r="N35">
+        <v>-66536.8940010074</v>
+      </c>
+    </row>
+    <row r="36" spans="6:14">
+      <c r="F36">
+        <v>40</v>
+      </c>
+      <c r="G36">
+        <v>-80909.477282258798</v>
+      </c>
+      <c r="I36">
+        <v>298102.295816964</v>
+      </c>
+      <c r="J36">
+        <v>40</v>
+      </c>
+      <c r="K36">
+        <v>298102.295816964</v>
+      </c>
+      <c r="M36">
+        <v>40</v>
+      </c>
+      <c r="N36">
+        <v>-80909.477282258798</v>
+      </c>
+    </row>
+    <row r="37" spans="6:14">
+      <c r="F37">
+        <v>41</v>
+      </c>
+      <c r="G37">
+        <v>-96614.062167079595</v>
+      </c>
+      <c r="I37">
+        <v>312586.15660199698</v>
+      </c>
+      <c r="J37">
+        <v>41</v>
+      </c>
+      <c r="K37">
+        <v>312586.15660199698</v>
+      </c>
+      <c r="M37">
+        <v>41</v>
+      </c>
+      <c r="N37">
+        <v>-96614.062167079595</v>
+      </c>
+    </row>
+    <row r="38" spans="6:14">
+      <c r="F38">
+        <v>42</v>
+      </c>
+      <c r="G38">
+        <v>-112894.46359497801</v>
+      </c>
+      <c r="I38">
+        <v>326844.98159125302</v>
+      </c>
+      <c r="J38">
+        <v>42</v>
+      </c>
+      <c r="K38">
+        <v>326844.98159125302</v>
+      </c>
+      <c r="M38">
+        <v>42</v>
+      </c>
+      <c r="N38">
+        <v>-112894.46359497801</v>
+      </c>
+    </row>
+    <row r="39" spans="6:14">
+      <c r="F39">
+        <v>43</v>
+      </c>
+      <c r="G39">
+        <v>-129707.855665275</v>
+      </c>
+      <c r="I39">
+        <v>341309.93414580199</v>
+      </c>
+      <c r="J39">
+        <v>43</v>
+      </c>
+      <c r="K39">
+        <v>341309.93414580199</v>
+      </c>
+      <c r="M39">
+        <v>43</v>
+      </c>
+      <c r="N39">
+        <v>-129707.855665275</v>
+      </c>
+    </row>
+    <row r="40" spans="6:14">
+      <c r="F40">
+        <v>45</v>
+      </c>
+      <c r="G40">
+        <v>-147000.746237521</v>
+      </c>
+      <c r="I40">
+        <v>356182.72409480799</v>
+      </c>
+      <c r="J40">
+        <v>45</v>
+      </c>
+      <c r="K40">
+        <v>356182.72409480897</v>
+      </c>
+      <c r="M40">
+        <v>45</v>
+      </c>
+      <c r="N40">
+        <v>-147000.746237521</v>
+      </c>
+    </row>
+    <row r="41" spans="6:14">
+      <c r="F41">
+        <v>46</v>
+      </c>
+      <c r="G41">
+        <v>-164469.85029438001</v>
+      </c>
+      <c r="I41">
+        <v>371152.73160628701</v>
+      </c>
+      <c r="J41">
+        <v>46</v>
+      </c>
+      <c r="K41">
+        <v>371152.73160628701</v>
+      </c>
+    </row>
+    <row r="42" spans="6:14">
+      <c r="F42">
+        <v>48</v>
+      </c>
+      <c r="G42">
+        <v>-181981.945784843</v>
+      </c>
+      <c r="I42">
+        <v>386402.09906171903</v>
+      </c>
+      <c r="J42">
+        <v>48</v>
+      </c>
+      <c r="K42">
+        <v>386402.09906171903</v>
+      </c>
+    </row>
+    <row r="43" spans="6:14">
+      <c r="F43">
+        <v>49</v>
+      </c>
+      <c r="G43">
+        <v>-199543.259396832</v>
+      </c>
+      <c r="I43">
+        <v>401884.03041093802</v>
+      </c>
+      <c r="J43">
+        <v>49</v>
+      </c>
+      <c r="K43">
+        <v>401884.03041093802</v>
+      </c>
+    </row>
+    <row r="44" spans="6:14">
+      <c r="F44">
+        <v>51</v>
+      </c>
+      <c r="G44">
+        <v>-217227.851626102</v>
+      </c>
+      <c r="I44">
+        <v>417811.43268141901</v>
+      </c>
+      <c r="J44">
+        <v>51</v>
+      </c>
+      <c r="K44">
+        <v>417811.43268142</v>
+      </c>
+    </row>
+    <row r="45" spans="6:14">
+      <c r="F45">
+        <v>52</v>
+      </c>
+      <c r="G45">
+        <v>-234600.315874341</v>
+      </c>
+      <c r="I45">
+        <v>433662.25259828899</v>
+      </c>
+      <c r="J45">
+        <v>52</v>
+      </c>
+      <c r="K45">
+        <v>433662.25259828899</v>
+      </c>
+    </row>
+    <row r="46" spans="6:14">
+      <c r="F46">
+        <v>54</v>
+      </c>
+      <c r="G46">
+        <v>-252275.583212695</v>
+      </c>
+      <c r="I46">
+        <v>450174.20068717998</v>
+      </c>
+      <c r="J46">
+        <v>54</v>
+      </c>
+      <c r="K46">
+        <v>450174.20068717998</v>
+      </c>
+    </row>
+    <row r="47" spans="6:14">
+      <c r="F47">
+        <v>55</v>
+      </c>
+      <c r="G47">
+        <v>-269658.99428038101</v>
+      </c>
+      <c r="I47">
+        <v>466749.44702776498</v>
+      </c>
+      <c r="J47">
+        <v>55</v>
+      </c>
+      <c r="K47">
+        <v>466749.44702776498</v>
+      </c>
+    </row>
+    <row r="48" spans="6:14">
+      <c r="F48">
+        <v>57</v>
+      </c>
+      <c r="G48">
+        <v>-287194.41108804301</v>
+      </c>
+      <c r="I48">
+        <v>483775.52398867498</v>
+      </c>
+      <c r="J48">
+        <v>57</v>
+      </c>
+      <c r="K48">
+        <v>483775.52398867498</v>
+      </c>
+    </row>
+    <row r="49" spans="6:11">
+      <c r="F49">
+        <v>58</v>
+      </c>
+      <c r="G49">
+        <v>-304904.03679663601</v>
+      </c>
+      <c r="I49">
+        <v>501150.31949682999</v>
+      </c>
+      <c r="J49">
+        <v>58</v>
+      </c>
+      <c r="K49">
+        <v>501150.31949682999</v>
+      </c>
+    </row>
+    <row r="50" spans="6:11">
+      <c r="F50">
+        <v>60</v>
+      </c>
+      <c r="G50">
+        <v>-322630.48594605702</v>
+      </c>
+      <c r="I50">
+        <v>518758.51355916099</v>
+      </c>
+      <c r="J50">
+        <v>60</v>
+      </c>
+      <c r="K50">
+        <v>518758.51355916099</v>
+      </c>
+    </row>
+    <row r="51" spans="6:11">
+      <c r="F51">
+        <v>61</v>
+      </c>
+      <c r="G51">
+        <v>-340398.62212343601</v>
+      </c>
+      <c r="I51">
+        <v>536550.09382952098</v>
+      </c>
+      <c r="J51">
+        <v>61</v>
+      </c>
+      <c r="K51">
+        <v>536550.09382952005</v>
+      </c>
+    </row>
+    <row r="52" spans="6:11">
+      <c r="F52">
+        <v>63</v>
+      </c>
+      <c r="G52">
+        <v>-358498.41961695702</v>
+      </c>
+      <c r="I52">
+        <v>554784.94751463202</v>
+      </c>
+      <c r="J52">
+        <v>63</v>
+      </c>
+      <c r="K52">
+        <v>554784.94751463202</v>
+      </c>
+    </row>
+    <row r="53" spans="6:11">
+      <c r="F53">
+        <v>64</v>
+      </c>
+      <c r="G53">
+        <v>-376311.716799177</v>
+      </c>
+      <c r="I53">
+        <v>572684.965078081</v>
+      </c>
+      <c r="J53">
+        <v>64</v>
+      </c>
+      <c r="K53">
+        <v>572684.96507807996</v>
+      </c>
+    </row>
+    <row r="54" spans="6:11">
+      <c r="F54">
+        <v>66</v>
+      </c>
+      <c r="G54">
+        <v>-394228.97905414097</v>
+      </c>
+      <c r="I54">
+        <v>590751.47774216905</v>
+      </c>
+      <c r="J54">
+        <v>66</v>
+      </c>
+      <c r="K54">
+        <v>590751.477742168</v>
+      </c>
+    </row>
+    <row r="55" spans="6:11">
+      <c r="F55">
+        <v>67</v>
+      </c>
+      <c r="G55">
+        <v>-412082.60444644402</v>
+      </c>
+      <c r="I55">
+        <v>608864.17020889802</v>
+      </c>
+      <c r="J55">
+        <v>67</v>
+      </c>
+      <c r="K55">
+        <v>608864.17020889698</v>
+      </c>
+    </row>
+    <row r="56" spans="6:11">
+      <c r="F56">
+        <v>69</v>
+      </c>
+      <c r="G56">
+        <v>-430173.94544888701</v>
+      </c>
+      <c r="I56">
+        <v>627285.62457147904</v>
+      </c>
+      <c r="J56">
+        <v>69</v>
+      </c>
+      <c r="K56">
+        <v>627285.62457147799</v>
+      </c>
+    </row>
+    <row r="57" spans="6:11">
+      <c r="H57">
+        <v>70</v>
+      </c>
+      <c r="I57">
+        <v>645618.38996980898</v>
+      </c>
+      <c r="J57">
+        <v>70</v>
+      </c>
+      <c r="K57">
+        <v>645618.38996980805</v>
+      </c>
+    </row>
+    <row r="58" spans="6:11">
+      <c r="H58">
+        <v>72</v>
+      </c>
+      <c r="I58">
+        <v>664133.52906700899</v>
+      </c>
+      <c r="J58">
+        <v>72</v>
+      </c>
+      <c r="K58">
+        <v>664133.52906700899</v>
+      </c>
+    </row>
+    <row r="59" spans="6:11">
+      <c r="H59">
+        <v>73</v>
+      </c>
+      <c r="I59">
+        <v>682712.74387429398</v>
+      </c>
+      <c r="J59">
+        <v>73</v>
+      </c>
+      <c r="K59">
+        <v>682712.74387429305</v>
+      </c>
+    </row>
+    <row r="60" spans="6:11">
+      <c r="H60">
+        <v>75</v>
+      </c>
+      <c r="I60">
+        <v>701487.36525202903</v>
+      </c>
+    </row>
+    <row r="61" spans="6:11">
+      <c r="H61">
+        <v>76</v>
+      </c>
+      <c r="I61">
+        <v>719868.19178418699</v>
+      </c>
+    </row>
+    <row r="62" spans="6:11">
+      <c r="H62">
+        <v>78</v>
+      </c>
+      <c r="I62">
+        <v>738462.55988291104</v>
+      </c>
+    </row>
+    <row r="63" spans="6:11">
+      <c r="H63">
+        <v>79</v>
+      </c>
+      <c r="I63">
+        <v>756732.95455184695</v>
+      </c>
+    </row>
+    <row r="64" spans="6:11">
+      <c r="H64">
+        <v>81</v>
+      </c>
+      <c r="I64">
+        <v>775562.21784167003</v>
+      </c>
+    </row>
+    <row r="65" spans="8:9">
+      <c r="H65">
+        <v>82</v>
+      </c>
+      <c r="I65">
+        <v>793621.55471796298</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="M1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>